<commit_message>
Product and Sprint Bakclog
No se por que siempre sale que los comitee, creo que es por que los abri
</commit_message>
<xml_diff>
--- a/documentacion/Product Backlog.xlsx
+++ b/documentacion/Product Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="18915" windowHeight="8445"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="18915" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>num</t>
   </si>
@@ -72,6 +72,9 @@
     <t>Estimacion inicial</t>
   </si>
   <si>
+    <t>Nueva Estimación por Sprint</t>
+  </si>
+  <si>
     <t>Product Backlog: Inventario</t>
   </si>
   <si>
@@ -79,22 +82,13 @@
   </si>
   <si>
     <t>Historia de Usuario</t>
-  </si>
-  <si>
-    <t>Estimación terminado el 1º Sprint</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESTIMACION POR PROGRESION DE FIBONACCI </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -147,6 +141,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -155,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -163,16 +170,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -186,18 +197,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -205,11 +209,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -288,7 +287,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -323,7 +321,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,14 +496,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
@@ -514,414 +511,307 @@
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2"/>
       <c r="B2" s="4"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
-      <c r="B4" s="5">
+      <c r="B4" s="8">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="9">
         <v>5</v>
       </c>
-      <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4" s="13">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3"/>
-      <c r="B5" s="5">
+      <c r="B5" s="8">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="9">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-      <c r="F5" s="13">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="3"/>
-      <c r="B6" s="5">
+      <c r="B6" s="8">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="9">
         <v>3</v>
       </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="13">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="3"/>
-      <c r="B7" s="5">
+      <c r="B7" s="8">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="9">
         <v>4</v>
       </c>
-      <c r="E7" s="1">
-        <v>5</v>
-      </c>
-      <c r="F7" s="13">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="3"/>
-      <c r="B8" s="5">
+      <c r="B8" s="8">
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="9">
         <v>2</v>
       </c>
-      <c r="E8" s="1">
-        <v>5</v>
-      </c>
-      <c r="F8" s="13">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="3"/>
-      <c r="B9" s="5">
+      <c r="B9" s="8">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="9">
         <v>5</v>
       </c>
-      <c r="E9" s="1">
-        <v>8</v>
-      </c>
-      <c r="F9" s="13">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="3"/>
-      <c r="B10" s="5">
+      <c r="B10" s="8">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="9">
         <v>6</v>
       </c>
-      <c r="E10" s="1">
-        <v>5</v>
-      </c>
-      <c r="F10" s="13">
-        <v>3</v>
-      </c>
-      <c r="G10" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="3"/>
-      <c r="B11" s="5">
+      <c r="B11" s="8">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="9">
         <v>7</v>
       </c>
-      <c r="E11" s="1">
-        <v>5</v>
-      </c>
-      <c r="F11" s="13">
-        <v>5</v>
-      </c>
-      <c r="G11" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
+      <c r="E11" s="1"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="6">
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="9">
         <v>8</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="1"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30">
+      <c r="B16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30">
+      <c r="B17" s="11">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="11">
         <v>2</v>
       </c>
-      <c r="F12" s="14">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="9">
-        <v>1</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="11">
-        <v>1</v>
-      </c>
-      <c r="E17" s="10">
-        <v>5</v>
-      </c>
-      <c r="F17" s="10">
+      <c r="C18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="13">
         <v>3</v>
       </c>
-      <c r="G17" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="9">
-        <v>2</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="11">
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="10">
-        <v>5</v>
-      </c>
-      <c r="F18" s="10">
+      <c r="C19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="13">
+        <v>4</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="11">
+        <v>4</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="13">
         <v>3</v>
       </c>
-      <c r="G18" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="9">
-        <v>3</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="11">
-        <v>4</v>
-      </c>
-      <c r="E19" s="10">
-        <v>3</v>
-      </c>
-      <c r="F19" s="10">
-        <v>1</v>
-      </c>
-      <c r="G19" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="9">
-        <v>4</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="11">
-        <v>3</v>
-      </c>
-      <c r="E20" s="10">
-        <v>2</v>
-      </c>
-      <c r="F20" s="10">
-        <v>1</v>
-      </c>
-      <c r="G20" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="2:7">
       <c r="G21" s="4"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C25" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="15">
-        <v>1</v>
-      </c>
-      <c r="E25" s="15">
-        <v>1</v>
-      </c>
-      <c r="F25" s="15">
-        <v>2</v>
-      </c>
-      <c r="G25" s="15">
-        <v>3</v>
-      </c>
-      <c r="H25" s="15">
-        <v>5</v>
-      </c>
-      <c r="I25" s="15">
-        <v>8</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>